<commit_message>
relation to saddle point & matrix definiteness criterion
</commit_message>
<xml_diff>
--- a/linear_forms.xlsx
+++ b/linear_forms.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>F</t>
   </si>
@@ -199,6 +199,39 @@
   </si>
   <si>
     <t>A =</t>
+  </si>
+  <si>
+    <t>A is transition matrix from base e to e'</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>f(x=[x1,x2])=ax1^2+2bx1x2+cx2^2</t>
+  </si>
+  <si>
+    <t>Quadratic form is positive if its diagonal coefficients in canonical form are all positive:</t>
+  </si>
+  <si>
+    <t>a=</t>
+  </si>
+  <si>
+    <t>c-b^2/a</t>
+  </si>
+  <si>
+    <t>F=</t>
+  </si>
+  <si>
+    <t>that is, iff:</t>
+  </si>
+  <si>
+    <t>a&gt;0 &amp; detF&gt;0</t>
   </si>
 </sst>
 </file>
@@ -611,14 +644,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:AA54"/>
+  <dimension ref="D4:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AB57" sqref="AB57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="22" max="22" width="12.28515625" customWidth="1"/>
     <col min="23" max="23" width="12.5703125" customWidth="1"/>
@@ -655,6 +689,12 @@
       <c r="J6" s="3">
         <v>2</v>
       </c>
+      <c r="K6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
       <c r="N6" t="s">
         <v>1</v>
       </c>
@@ -693,6 +733,12 @@
       <c r="J7" s="3">
         <v>1</v>
       </c>
+      <c r="K7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" t="s">
+        <v>64</v>
+      </c>
       <c r="O7">
         <v>1.5</v>
       </c>
@@ -766,6 +812,9 @@
       <c r="J14">
         <f>-I7/I6</f>
         <v>-2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="4:27" x14ac:dyDescent="0.25">
@@ -1221,7 +1270,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D50" s="8" t="s">
         <v>53</v>
       </c>
@@ -1238,7 +1287,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D51" s="8"/>
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
@@ -1246,12 +1295,32 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="Q52" t="s">
+        <v>69</v>
+      </c>
+      <c r="R52" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="S52" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T52" s="3">
+        <f>I6</f>
+        <v>1</v>
+      </c>
+      <c r="U52" s="3">
+        <f>J6</f>
+        <v>2</v>
+      </c>
+      <c r="V52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D53" s="8" t="s">
         <v>56</v>
       </c>
@@ -1267,13 +1336,68 @@
       <c r="J53" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="R53" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="S53" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="T53" s="3">
+        <f>I7</f>
+        <v>2</v>
+      </c>
+      <c r="U53" s="3">
+        <f>J7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D54" s="8"/>
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
       <c r="J54" t="s">
         <v>58</v>
+      </c>
+      <c r="V54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="V55">
+        <f>T52</f>
+        <v>1</v>
+      </c>
+      <c r="W55">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z55">
+        <f>V55</f>
+        <v>1</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <f>U53-(U52^2)/T52</f>
+        <v>-3</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z56">
+        <f>W56</f>
+        <v>-3</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>